<commit_message>
fix: correct translation for December in Portuguese locale
</commit_message>
<xml_diff>
--- a/backend/data/climatologias_SOLAR.xlsx
+++ b/backend/data/climatologias_SOLAR.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Nov</t>
   </si>
   <si>
-    <t xml:space="preserve">Dez</t>
+    <t xml:space="preserve">Dec</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>